<commit_message>
Added tag list import for fund formulas
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_formulas.xlsx
+++ b/public/sample_uploads/fund_formulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43BD8B2-CB67-4711-8C92-84A11953B001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA96F1D-6515-4ADC-BBE2-CDA2B54A2732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FundFormula" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Sequence</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>Interest</t>
+  </si>
+  <si>
+    <t>Tag List</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
   </si>
 </sst>
 </file>
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E5" sqref="E5:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -491,14 +500,15 @@
     <col min="2" max="2" width="45.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.8125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.8125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3125" customWidth="1"/>
+    <col min="6" max="6" width="19.8125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,22 +522,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -541,22 +554,25 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -570,22 +586,25 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -599,22 +618,25 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -628,22 +650,25 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -657,22 +682,25 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
@@ -686,22 +714,25 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -715,22 +746,25 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -744,22 +778,25 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -773,18 +810,21 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
       <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ytd quarterly allocations (#702)
* Added Generate YTD, Quarterly, Since Inception numbers, to fund formulas

* Refactored AccountEntryAllocationEngine to Engine

* Fixed CRP import tests

* Backup

* Refactored Engine

* Refactored Engine

* Relocated the ALlocations Engine to the right directory

* Added YTD, Quarterly etc

* Changed the names of AE generated for YTD Quarter etc

* Changed the names of AE generated for YTD Quarter etc

* Fixed issue with YTD change

* Fixed issue with YTD change

* Backup

* Moved commitment cache to the new engine

* Changed uniq index for account_entry to enable rollups

* Now deletes all cumulative account entries before a run

* Now deletes all account entries before a run

* Fixed bulk insert count check

* Fixed commitment_type of cumulative account entry

* Fixed upload and download for fund formulas

* Misc fixes

* Fixed SkipRule

* Added fund rollups for ytd qty etc

* Added fund rollups for ytd qty etc

* Fixed import of Fund formulas
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_formulas.xlsx
+++ b/public/sample_uploads/fund_formulas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA96F1D-6515-4ADC-BBE2-CDA2B54A2732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9749C628-08D4-4BB5-9178-EC3AB6338B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
   <si>
     <t>Sequence</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Generate YTD, Quarterly, Since Inception numbers</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -500,15 +509,15 @@
     <col min="2" max="2" width="45.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.8125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3125" customWidth="1"/>
-    <col min="6" max="6" width="19.8125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.3125" customWidth="1"/>
+    <col min="7" max="7" width="19.8125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,25 +531,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -554,25 +566,28 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -586,25 +601,28 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -618,25 +636,28 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
       <c r="J4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -650,25 +671,28 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
       <c r="J5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -682,25 +706,28 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
       <c r="J6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>7</v>
       </c>
@@ -714,25 +741,28 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
       <c r="J7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -746,25 +776,28 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
       <c r="J8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -778,25 +811,28 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -810,21 +846,24 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
       <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added spec for formula upload, updated excel
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_formulas.xlsx
+++ b/public/sample_uploads/fund_formulas.xlsx
@@ -70,8 +70,7 @@
     <t xml:space="preserve">Monthly</t>
   </si>
   <si>
-    <t xml:space="preserve">capital_commitment.committed_amount_cents * ( fund_unit_setting.management_fee / 4 ) / 100	
-</t>
+    <t xml:space="preserve">capital_commitment.committed_amount_cents * ( fund_unit_setting.management_fee / 4 ) / 100</t>
   </si>
   <si>
     <t xml:space="preserve">Fees</t>
@@ -98,7 +97,7 @@
     <t xml:space="preserve">Quarterly</t>
   </si>
   <si>
-    <t xml:space="preserve">capital_commitment.fund.total_units_premium_cents * capital_commitment.percentage  / 100	</t>
+    <t xml:space="preserve">capital_commitment.fund.total_units_premium_cents * capital_commitment.percentage / 100</t>
   </si>
   <si>
     <t xml:space="preserve">Premium</t>
@@ -110,7 +109,7 @@
     <t xml:space="preserve">Generate Investable Capital</t>
   </si>
   <si>
-    <t xml:space="preserve">capital_commitment["properties"]["investable_capital"] = ( capital_commitment.collected_amount_cents - capital_commitment.cumulative_account_entry("Management Fees").amount_cents  + capital_commitment.cumulative_account_entry("Unit Premium").amount_cents )  / 100</t>
+    <t xml:space="preserve">capital_commitment["properties"]["investable_capital"] = ( capital_commitment.collected_amount_cents - capital_commitment.cumulative_account_entry("Management Fees").amount_cents + capital_commitment.cumulative_account_entry("Unit Premium").amount_cents ) / 100</t>
   </si>
   <si>
     <t xml:space="preserve">Capital</t>
@@ -128,8 +127,7 @@
     <t xml:space="preserve">Accured Interest</t>
   </si>
   <si>
-    <t xml:space="preserve">fund_account_entry.amount_cents * capital_commitment.properties['investable_capital_percentage']  / 100.0	
-</t>
+    <t xml:space="preserve">fund_account_entry.amount_cents * capital_commitment.properties['investable_capital_percentage'] / 100.0</t>
   </si>
   <si>
     <t xml:space="preserve">Interest</t>
@@ -232,16 +230,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,374 +438,374 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="255"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="255"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="b">
+      <c r="J2" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="b">
+      <c r="J3" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="b">
+      <c r="J4" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="b">
+      <c r="J5" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="2" t="b">
+      <c r="J6" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="b">
+      <c r="J7" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="b">
+      <c r="J8" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="b">
+      <c r="J9" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="b">
+      <c r="J10" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>